<commit_message>
pruebas con excel OCA.SUM.CLINICA realizadas + agregación de carpeta DOM
</commit_message>
<xml_diff>
--- a/excel/OCA.xlsx
+++ b/excel/OCA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A69729-8F72-465F-B3DA-9DA89B608D81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1114F142-8BE4-46E1-8EE1-F660984844F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="3900" windowWidth="20190" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20190" windowHeight="10140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="48">
   <si>
     <t>idAlumno</t>
   </si>
@@ -141,16 +141,34 @@
     <t>bbbbb</t>
   </si>
   <si>
-    <t>igermi@unmsm.edu.pe</t>
-  </si>
-  <si>
-    <t>gales@unmsm.edu.pe</t>
-  </si>
-  <si>
     <t>xxxxx</t>
   </si>
   <si>
     <t>yyyy</t>
+  </si>
+  <si>
+    <t>e@unmsm.edu.pe</t>
+  </si>
+  <si>
+    <t>a@unmsm.edu.pe</t>
+  </si>
+  <si>
+    <t>b@unmsm.edu.pe</t>
+  </si>
+  <si>
+    <t>c@unmsm.edu.pe</t>
+  </si>
+  <si>
+    <t>d@unmsm.edu.pe</t>
+  </si>
+  <si>
+    <t>aaaaa</t>
+  </si>
+  <si>
+    <t>bbbb</t>
+  </si>
+  <si>
+    <t>jsjsjs</t>
   </si>
 </sst>
 </file>
@@ -480,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:Z6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:W1048576"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +641,7 @@
         <v>14</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K2">
         <v>15</v>
@@ -656,7 +674,7 @@
         <v>36</v>
       </c>
       <c r="U2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="V2" t="s">
         <v>36</v>
@@ -703,7 +721,7 @@
         <v>14</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="K3">
         <v>16</v>
@@ -736,7 +754,7 @@
         <v>37</v>
       </c>
       <c r="U3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="V3" t="s">
         <v>37</v>
@@ -752,12 +770,255 @@
       </c>
       <c r="Z3" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>16200277</v>
+      </c>
+      <c r="B4">
+        <v>71395616</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1">
+        <v>35953</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K4">
+        <v>17</v>
+      </c>
+      <c r="L4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>36</v>
+      </c>
+      <c r="R4" t="s">
+        <v>36</v>
+      </c>
+      <c r="S4" t="s">
+        <v>36</v>
+      </c>
+      <c r="T4" t="s">
+        <v>36</v>
+      </c>
+      <c r="U4" t="s">
+        <v>38</v>
+      </c>
+      <c r="V4" t="s">
+        <v>36</v>
+      </c>
+      <c r="W4" t="s">
+        <v>36</v>
+      </c>
+      <c r="X4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>16200278</v>
+      </c>
+      <c r="B5">
+        <v>71395617</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="1">
+        <v>35953</v>
+      </c>
+      <c r="I5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K5">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R5" t="s">
+        <v>37</v>
+      </c>
+      <c r="S5" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U5" t="s">
+        <v>39</v>
+      </c>
+      <c r="V5" t="s">
+        <v>37</v>
+      </c>
+      <c r="W5" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>16200279</v>
+      </c>
+      <c r="B6">
+        <v>71395618</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="1">
+        <v>35953</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K6">
+        <v>19</v>
+      </c>
+      <c r="L6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S6" t="s">
+        <v>36</v>
+      </c>
+      <c r="T6" t="s">
+        <v>36</v>
+      </c>
+      <c r="U6" t="s">
+        <v>38</v>
+      </c>
+      <c r="V6" t="s">
+        <v>36</v>
+      </c>
+      <c r="W6" t="s">
+        <v>36</v>
+      </c>
+      <c r="X6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" xr:uid="{DD1FC96F-F7FC-475C-A888-2AA3BF7186D5}"/>
     <hyperlink ref="J3" r:id="rId2" xr:uid="{0455F4B8-76B4-4EB5-9C84-788618CA8E83}"/>
+    <hyperlink ref="J4" r:id="rId3" xr:uid="{3C097BB9-DE38-4CA7-A8FF-115A0F28E6A0}"/>
+    <hyperlink ref="J6" r:id="rId4" xr:uid="{DE77267D-D4B3-4CE1-B7C7-B85487F0FED9}"/>
+    <hyperlink ref="J5" r:id="rId5" xr:uid="{9B7BB57D-B1CB-4A82-B212-B21B5E5FBA01}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>